<commit_message>
Added background books for recommendations + dissertations
</commit_message>
<xml_diff>
--- a/src/data/topic_polygons.xlsx
+++ b/src/data/topic_polygons.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A001706-7F8C-4A34-A0DA-765D4DB147C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF8705-2119-4BF5-B8DF-2E1CA427E298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{947AC799-C70E-4069-BD4E-C9549BB2958C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="37">
   <si>
     <t>topic</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>topic_3</t>
+  </si>
+  <si>
+    <t>recommended_books</t>
+  </si>
+  <si>
+    <t>student_work</t>
+  </si>
+  <si>
+    <t>heritage_objects</t>
+  </si>
+  <si>
+    <t>dissertations</t>
   </si>
 </sst>
 </file>
@@ -515,16 +527,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F13559-951A-47A0-A686-1C942B342977}">
-  <dimension ref="A1:R109"/>
+  <dimension ref="A1:R125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K112" sqref="K112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.08984375" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="6" width="8.7265625" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="6" width="8.7265625" customWidth="1" outlineLevel="1"/>
     <col min="7" max="8" width="15.08984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3646,6 +3661,454 @@
         <v>0.771608986573315</v>
       </c>
     </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>33</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110">
+        <v>231.042</v>
+      </c>
+      <c r="D110">
+        <v>182.26900000000001</v>
+      </c>
+      <c r="E110">
+        <v>1002.816</v>
+      </c>
+      <c r="F110">
+        <v>225.67</v>
+      </c>
+      <c r="G110" s="1">
+        <f t="shared" ref="G110:G113" si="19">C110/E110</f>
+        <v>0.23039321271300017</v>
+      </c>
+      <c r="H110" s="1">
+        <f t="shared" ref="H110:H113" si="20">D110/F110</f>
+        <v>0.8076793548101211</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>33</v>
+      </c>
+      <c r="B111">
+        <v>2</v>
+      </c>
+      <c r="C111">
+        <v>268.84300000000002</v>
+      </c>
+      <c r="D111">
+        <v>182.26900000000001</v>
+      </c>
+      <c r="E111">
+        <v>1002.816</v>
+      </c>
+      <c r="F111">
+        <v>225.67</v>
+      </c>
+      <c r="G111" s="1">
+        <f t="shared" si="19"/>
+        <v>0.26808806401174295</v>
+      </c>
+      <c r="H111" s="1">
+        <f t="shared" si="20"/>
+        <v>0.8076793548101211</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>33</v>
+      </c>
+      <c r="B112">
+        <v>3</v>
+      </c>
+      <c r="C112">
+        <v>268.84300000000002</v>
+      </c>
+      <c r="D112">
+        <v>201.17099999999999</v>
+      </c>
+      <c r="E112">
+        <v>1002.816</v>
+      </c>
+      <c r="F112">
+        <v>225.67</v>
+      </c>
+      <c r="G112" s="1">
+        <f t="shared" si="19"/>
+        <v>0.26808806401174295</v>
+      </c>
+      <c r="H112" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89143882660522</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>33</v>
+      </c>
+      <c r="B113">
+        <v>4</v>
+      </c>
+      <c r="C113">
+        <v>231.04300000000001</v>
+      </c>
+      <c r="D113">
+        <v>201.17099999999999</v>
+      </c>
+      <c r="E113">
+        <v>1002.816</v>
+      </c>
+      <c r="F113">
+        <v>225.67</v>
+      </c>
+      <c r="G113" s="1">
+        <f t="shared" si="19"/>
+        <v>0.23039420990490778</v>
+      </c>
+      <c r="H113" s="1">
+        <f t="shared" si="20"/>
+        <v>0.89143882660522</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>34</v>
+      </c>
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114">
+        <v>116.423</v>
+      </c>
+      <c r="D114">
+        <v>145.59700000000001</v>
+      </c>
+      <c r="E114">
+        <v>1002.816</v>
+      </c>
+      <c r="F114">
+        <v>225.67</v>
+      </c>
+      <c r="G114" s="1">
+        <f t="shared" ref="G114:G117" si="21">C114/E114</f>
+        <v>0.11609607345714468</v>
+      </c>
+      <c r="H114" s="1">
+        <f t="shared" ref="H114:H117" si="22">D114/F114</f>
+        <v>0.64517658527939037</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>34</v>
+      </c>
+      <c r="B115">
+        <v>2</v>
+      </c>
+      <c r="C115">
+        <v>154.22800000000001</v>
+      </c>
+      <c r="D115">
+        <v>145.59700000000001</v>
+      </c>
+      <c r="E115">
+        <v>1002.816</v>
+      </c>
+      <c r="F115">
+        <v>225.67</v>
+      </c>
+      <c r="G115" s="1">
+        <f t="shared" si="21"/>
+        <v>0.15379491352351779</v>
+      </c>
+      <c r="H115" s="1">
+        <f t="shared" si="22"/>
+        <v>0.64517658527939037</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>34</v>
+      </c>
+      <c r="B116">
+        <v>3</v>
+      </c>
+      <c r="C116">
+        <v>154.22800000000001</v>
+      </c>
+      <c r="D116">
+        <v>174.12799999999999</v>
+      </c>
+      <c r="E116">
+        <v>1002.816</v>
+      </c>
+      <c r="F116">
+        <v>225.67</v>
+      </c>
+      <c r="G116" s="1">
+        <f t="shared" si="21"/>
+        <v>0.15379491352351779</v>
+      </c>
+      <c r="H116" s="1">
+        <f t="shared" si="22"/>
+        <v>0.77160455532414585</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B117">
+        <v>4</v>
+      </c>
+      <c r="C117">
+        <v>116.423</v>
+      </c>
+      <c r="D117">
+        <v>174.12799999999999</v>
+      </c>
+      <c r="E117">
+        <v>1002.816</v>
+      </c>
+      <c r="F117">
+        <v>225.67</v>
+      </c>
+      <c r="G117" s="1">
+        <f t="shared" si="21"/>
+        <v>0.11609607345714468</v>
+      </c>
+      <c r="H117" s="1">
+        <f t="shared" si="22"/>
+        <v>0.77160455532414585</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>35</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+      <c r="C118">
+        <v>728.12</v>
+      </c>
+      <c r="D118">
+        <v>182.41200000000001</v>
+      </c>
+      <c r="E118">
+        <v>1002.816</v>
+      </c>
+      <c r="F118">
+        <v>225.67</v>
+      </c>
+      <c r="G118" s="1">
+        <f t="shared" ref="G118:G125" si="23">C118/E118</f>
+        <v>0.72607537175314318</v>
+      </c>
+      <c r="H118" s="1">
+        <f t="shared" ref="H118:H125" si="24">D118/F118</f>
+        <v>0.80831302344130818</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>35</v>
+      </c>
+      <c r="B119">
+        <v>2</v>
+      </c>
+      <c r="C119">
+        <v>765.923</v>
+      </c>
+      <c r="D119">
+        <v>182.41200000000001</v>
+      </c>
+      <c r="E119">
+        <v>1002.816</v>
+      </c>
+      <c r="F119">
+        <v>225.67</v>
+      </c>
+      <c r="G119" s="1">
+        <f t="shared" si="23"/>
+        <v>0.76377221743570101</v>
+      </c>
+      <c r="H119" s="1">
+        <f t="shared" si="24"/>
+        <v>0.80831302344130818</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>35</v>
+      </c>
+      <c r="B120">
+        <v>3</v>
+      </c>
+      <c r="C120">
+        <v>765.923</v>
+      </c>
+      <c r="D120">
+        <v>210.94300000000001</v>
+      </c>
+      <c r="E120">
+        <v>1002.816</v>
+      </c>
+      <c r="F120">
+        <v>225.67</v>
+      </c>
+      <c r="G120" s="1">
+        <f t="shared" si="23"/>
+        <v>0.76377221743570101</v>
+      </c>
+      <c r="H120" s="1">
+        <f t="shared" si="24"/>
+        <v>0.93474099348606388</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>35</v>
+      </c>
+      <c r="B121">
+        <v>4</v>
+      </c>
+      <c r="C121">
+        <v>728.12</v>
+      </c>
+      <c r="D121">
+        <v>210.94300000000001</v>
+      </c>
+      <c r="E121">
+        <v>1002.816</v>
+      </c>
+      <c r="F121">
+        <v>225.67</v>
+      </c>
+      <c r="G121" s="1">
+        <f t="shared" si="23"/>
+        <v>0.72607537175314318</v>
+      </c>
+      <c r="H121" s="1">
+        <f t="shared" si="24"/>
+        <v>0.93474099348606388</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>36</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+      <c r="C122">
+        <v>766.27700000000004</v>
+      </c>
+      <c r="D122">
+        <v>182.41200000000001</v>
+      </c>
+      <c r="E122">
+        <v>1002.816</v>
+      </c>
+      <c r="F122">
+        <v>225.67</v>
+      </c>
+      <c r="G122" s="1">
+        <f t="shared" si="23"/>
+        <v>0.76412522337098732</v>
+      </c>
+      <c r="H122" s="1">
+        <f t="shared" si="24"/>
+        <v>0.80831302344130818</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>36</v>
+      </c>
+      <c r="B123">
+        <v>2</v>
+      </c>
+      <c r="C123">
+        <v>816.81600000000003</v>
+      </c>
+      <c r="D123">
+        <v>182.41200000000001</v>
+      </c>
+      <c r="E123">
+        <v>1002.816</v>
+      </c>
+      <c r="F123">
+        <v>225.67</v>
+      </c>
+      <c r="G123" s="1">
+        <f t="shared" si="23"/>
+        <v>0.81452230518858892</v>
+      </c>
+      <c r="H123" s="1">
+        <f t="shared" si="24"/>
+        <v>0.80831302344130818</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>36</v>
+      </c>
+      <c r="B124">
+        <v>3</v>
+      </c>
+      <c r="C124">
+        <v>816.81600000000003</v>
+      </c>
+      <c r="D124">
+        <v>210.94300000000001</v>
+      </c>
+      <c r="E124">
+        <v>1002.816</v>
+      </c>
+      <c r="F124">
+        <v>225.67</v>
+      </c>
+      <c r="G124" s="1">
+        <f t="shared" si="23"/>
+        <v>0.81452230518858892</v>
+      </c>
+      <c r="H124" s="1">
+        <f t="shared" si="24"/>
+        <v>0.93474099348606388</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>36</v>
+      </c>
+      <c r="B125">
+        <v>4</v>
+      </c>
+      <c r="C125">
+        <v>766.27700000000004</v>
+      </c>
+      <c r="D125">
+        <v>210.94300000000001</v>
+      </c>
+      <c r="E125">
+        <v>1002.816</v>
+      </c>
+      <c r="F125">
+        <v>225.67</v>
+      </c>
+      <c r="G125" s="1">
+        <f t="shared" si="23"/>
+        <v>0.76412522337098732</v>
+      </c>
+      <c r="H125" s="1">
+        <f t="shared" si="24"/>
+        <v>0.93474099348606388</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H109" xr:uid="{51F13559-951A-47A0-A686-1C942B342977}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrated animation for recommendations + dissertation
</commit_message>
<xml_diff>
--- a/src/data/topic_polygons.xlsx
+++ b/src/data/topic_polygons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEF8705-2119-4BF5-B8DF-2E1CA427E298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1379BC-2591-4271-A808-C1D4FE3AE534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{947AC799-C70E-4069-BD4E-C9549BB2958C}"/>
   </bookViews>
@@ -531,16 +531,17 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K112" sqref="K112"/>
+      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="7.81640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="6" width="8.7265625" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="8" width="15.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="7.81640625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="6" width="8.7265625" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="15.08984375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.08984375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Created screens for heritage + student work
</commit_message>
<xml_diff>
--- a/src/data/topic_polygons.xlsx
+++ b/src/data/topic_polygons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1379BC-2591-4271-A808-C1D4FE3AE534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C29034-107B-419C-B9DA-939B74E2F743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{947AC799-C70E-4069-BD4E-C9549BB2958C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$125</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -530,8 +530,8 @@
   <dimension ref="A1:R125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -4111,7 +4111,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H109" xr:uid="{51F13559-951A-47A0-A686-1C942B342977}"/>
+  <autoFilter ref="A1:H125" xr:uid="{51F13559-951A-47A0-A686-1C942B342977}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added study books. Fixed #13.
</commit_message>
<xml_diff>
--- a/src/data/topic_polygons.xlsx
+++ b/src/data/topic_polygons.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C29034-107B-419C-B9DA-939B74E2F743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7D4FC9-CCDA-4344-91D7-FAEDD551DB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{947AC799-C70E-4069-BD4E-C9549BB2958C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="38">
   <si>
     <t>topic</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>dissertations</t>
+  </si>
+  <si>
+    <t>study_books</t>
   </si>
 </sst>
 </file>
@@ -527,11 +530,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F13559-951A-47A0-A686-1C942B342977}">
-  <dimension ref="A1:R125"/>
+  <dimension ref="A1:R129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L123" sqref="L123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -3962,11 +3965,11 @@
         <v>225.67</v>
       </c>
       <c r="G120" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="G120:G129" si="25">C120/E120</f>
         <v>0.76377221743570101</v>
       </c>
       <c r="H120" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="H120:H129" si="26">D120/F120</f>
         <v>0.93474099348606388</v>
       </c>
     </row>
@@ -3990,11 +3993,11 @@
         <v>225.67</v>
       </c>
       <c r="G121" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.72607537175314318</v>
       </c>
       <c r="H121" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.93474099348606388</v>
       </c>
     </row>
@@ -4018,11 +4021,11 @@
         <v>225.67</v>
       </c>
       <c r="G122" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.76412522337098732</v>
       </c>
       <c r="H122" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.80831302344130818</v>
       </c>
     </row>
@@ -4046,11 +4049,11 @@
         <v>225.67</v>
       </c>
       <c r="G123" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.81452230518858892</v>
       </c>
       <c r="H123" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.80831302344130818</v>
       </c>
     </row>
@@ -4074,11 +4077,11 @@
         <v>225.67</v>
       </c>
       <c r="G124" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.81452230518858892</v>
       </c>
       <c r="H124" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.93474099348606388</v>
       </c>
     </row>
@@ -4102,11 +4105,123 @@
         <v>225.67</v>
       </c>
       <c r="G125" s="1">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.76412522337098732</v>
       </c>
       <c r="H125" s="1">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
+        <v>0.93474099348606388</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>37</v>
+      </c>
+      <c r="B126">
+        <v>1</v>
+      </c>
+      <c r="C126">
+        <v>626.17200000000003</v>
+      </c>
+      <c r="D126">
+        <v>182.411</v>
+      </c>
+      <c r="E126">
+        <v>1002.816</v>
+      </c>
+      <c r="F126">
+        <v>225.67</v>
+      </c>
+      <c r="G126" s="1">
+        <f t="shared" si="25"/>
+        <v>0.62441365115833813</v>
+      </c>
+      <c r="H126" s="1">
+        <f t="shared" si="26"/>
+        <v>0.80830859219213902</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>37</v>
+      </c>
+      <c r="B127">
+        <v>2</v>
+      </c>
+      <c r="C127">
+        <v>714.94899999999996</v>
+      </c>
+      <c r="D127">
+        <v>182.411</v>
+      </c>
+      <c r="E127">
+        <v>1002.816</v>
+      </c>
+      <c r="F127">
+        <v>225.67</v>
+      </c>
+      <c r="G127" s="1">
+        <f t="shared" si="25"/>
+        <v>0.71294135713829854</v>
+      </c>
+      <c r="H127" s="1">
+        <f t="shared" si="26"/>
+        <v>0.80830859219213902</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>37</v>
+      </c>
+      <c r="B128">
+        <v>3</v>
+      </c>
+      <c r="C128">
+        <v>714.94899999999996</v>
+      </c>
+      <c r="D128">
+        <v>210.94300000000001</v>
+      </c>
+      <c r="E128">
+        <v>1002.816</v>
+      </c>
+      <c r="F128">
+        <v>225.67</v>
+      </c>
+      <c r="G128" s="1">
+        <f t="shared" si="25"/>
+        <v>0.71294135713829854</v>
+      </c>
+      <c r="H128" s="1">
+        <f t="shared" si="26"/>
+        <v>0.93474099348606388</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>37</v>
+      </c>
+      <c r="B129">
+        <v>4</v>
+      </c>
+      <c r="C129">
+        <v>626.17200000000003</v>
+      </c>
+      <c r="D129">
+        <v>210.94300000000001</v>
+      </c>
+      <c r="E129">
+        <v>1002.816</v>
+      </c>
+      <c r="F129">
+        <v>225.67</v>
+      </c>
+      <c r="G129" s="1">
+        <f t="shared" si="25"/>
+        <v>0.62441365115833813</v>
+      </c>
+      <c r="H129" s="1">
+        <f t="shared" si="26"/>
         <v>0.93474099348606388</v>
       </c>
     </row>

</xml_diff>